<commit_message>
mp5 adjustments + a2 buff
</commit_message>
<xml_diff>
--- a/changes/mp5.xlsx
+++ b/changes/mp5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC2B76-0B70-49AC-B80A-01A17EBCEDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DF60C4-7CD9-4FF0-B967-727B97318611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>new</t>
   </si>
@@ -114,6 +114,48 @@
   </si>
   <si>
     <t>Surefire 628LMF-B MP5 Handguard</t>
+  </si>
+  <si>
+    <t>hk_mp5a3_early_gen_stock_endplate</t>
+  </si>
+  <si>
+    <t>HK MP5A3 Early Generation Stock Endplate</t>
+  </si>
+  <si>
+    <t>hk_mp5a3_early_gen_collapsible_stock</t>
+  </si>
+  <si>
+    <t>HK MP5A3 Early Generation Collapsible Stock</t>
+  </si>
+  <si>
+    <t>hk_mp5a2_plastic_fixed_stock</t>
+  </si>
+  <si>
+    <t>HK MP5A2 Plastic Fixed Stock</t>
+  </si>
+  <si>
+    <t>hk_mp5_hk94_stock_endcap</t>
+  </si>
+  <si>
+    <t>HP MP5/HK94 Stock Endcap</t>
+  </si>
+  <si>
+    <t>hk_mp5_endcap_sling_swivel</t>
+  </si>
+  <si>
+    <t>HK MP5 Endcap Sling Swivel</t>
+  </si>
+  <si>
+    <t>hk_mp5_hk94_choate_stock_base</t>
+  </si>
+  <si>
+    <t>HK MP5/HK94 Choate Stock Base</t>
+  </si>
+  <si>
+    <t>hk_mp5_hk94_choate_stock</t>
+  </si>
+  <si>
+    <t>HK MP5/HK94 Choate Stock</t>
   </si>
 </sst>
 </file>
@@ -958,12 +1000,12 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="22" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1085,7 +1127,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N9" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <f t="shared" ref="N4:N17" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
         <v>0</v>
       </c>
     </row>
@@ -1268,77 +1310,126 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-12</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0.08</v>
+      </c>
+      <c r="M12">
+        <v>1500</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999991</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>0.12</v>
+      </c>
+      <c r="E13">
+        <v>-9</v>
+      </c>
+      <c r="F13">
+        <v>-8</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>18.600000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0.06</v>
+      </c>
+      <c r="M14">
+        <v>1000</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.06</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1347,40 +1438,81 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="M15" s="1">
+        <v>750</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.2</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E16" s="1">
+        <v>-8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-13</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>10</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>0.2</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="M17" s="1">
+        <v>250</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>-5.1999999999999993</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
fix some minor stuff
</commit_message>
<xml_diff>
--- a/changes/mp5.xlsx
+++ b/changes/mp5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54BEA52-CAE1-4141-9BEB-4F11FBFCADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA48152-32F1-43AE-9072-3F7E55364DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,7 +994,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1108,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="E5" s="1">
         <v>-9</v>
@@ -1126,8 +1126,8 @@
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" ref="N4:N17" si="0">C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*10+J5/300</f>
-        <v>15.399999999999999</v>
+        <f t="shared" ref="N5:N17" si="0">C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*10+J5/300</f>
+        <v>15.8</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1138,10 +1138,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="E6" s="1">
         <v>-6</v>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
-        <v>14.8</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="E7" s="1">
         <v>-7</v>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
-        <v>15.6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="E8" s="1">
         <v>-9</v>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="1">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="E9" s="1">
         <v>-6</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>14.600000000000001</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>